<commit_message>
update the content of mvp
</commit_message>
<xml_diff>
--- a/doc/pchain开发计划.xlsx
+++ b/doc/pchain开发计划.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B56F3419-C6F2-4BC7-B464-2D0E69D232CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="7740" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="7740" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="正在进行或后续工作" sheetId="1" state="hidden" r:id="rId1"/>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="146">
   <si>
     <t>1,减小网络开销共识机制</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -615,12 +616,23 @@
     <t>初步制定测试用例</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve">    mvp 录制展示3个大的模块：
+    1, 共识 （由 张锐、赵路 提供用例）
+       内容：目前包含 reward scheme/epoch，validator 操作，validator与token账号挂钩，网络高效共识
+    2，smart data（由 侯冠豪 提供用例）
+       内容：evm添加新的指令，在 pchain 和 智能合约之间传递智能数据
+    3，安全（由 寅 教授提供内容）
+       内容：pchain的（加密）安全与防御机制
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -669,6 +681,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -710,7 +730,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -744,6 +764,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -756,11 +779,19 @@
       <color rgb="FF3333FF"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -802,7 +833,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -834,9 +865,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -868,6 +917,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1043,25 +1110,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C5:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="41.875" customWidth="1"/>
     <col min="7" max="7" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="3:7">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.15">
       <c r="D6" t="s">
         <v>1</v>
       </c>
@@ -1072,7 +1139,7 @@
         <v>3.28</v>
       </c>
     </row>
-    <row r="7" spans="3:7">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.15">
       <c r="D7" t="s">
         <v>3</v>
       </c>
@@ -1086,12 +1153,12 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="8" spans="3:7">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="3:7">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.15">
       <c r="D9" t="s">
         <v>5</v>
       </c>
@@ -1102,12 +1169,12 @@
         <v>3.28</v>
       </c>
     </row>
-    <row r="10" spans="3:7">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="3:7">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.15">
       <c r="D11" t="s">
         <v>8</v>
       </c>
@@ -1118,12 +1185,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="3:7">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="3:7">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.15">
       <c r="D13" t="s">
         <v>30</v>
       </c>
@@ -1134,12 +1201,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="3:7">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="3:7">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.15">
       <c r="D15" t="s">
         <v>13</v>
       </c>
@@ -1150,12 +1217,12 @@
         <v>3.28</v>
       </c>
     </row>
-    <row r="16" spans="3:7">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.15">
       <c r="D17" s="4" t="s">
         <v>16</v>
       </c>
@@ -1167,7 +1234,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="3:7">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.15">
       <c r="D18" s="4" t="s">
         <v>17</v>
       </c>
@@ -1179,7 +1246,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="3:7">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.15">
       <c r="D19" t="s">
         <v>18</v>
       </c>
@@ -1190,23 +1257,23 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="3:7">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.15">
       <c r="D21" t="s">
         <v>24</v>
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.15">
       <c r="D23" t="s">
         <v>26</v>
       </c>
@@ -1217,7 +1284,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.15">
       <c r="D24" t="s">
         <v>27</v>
       </c>
@@ -1228,12 +1295,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="3:7">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.15">
       <c r="D26" t="s">
         <v>29</v>
       </c>
@@ -1247,16 +1314,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="E6:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="6" spans="5:9">
+    <row r="6" spans="5:9" x14ac:dyDescent="0.15">
       <c r="E6" t="s">
         <v>31</v>
       </c>
@@ -1264,7 +1331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="5:9">
+    <row r="7" spans="5:9" x14ac:dyDescent="0.15">
       <c r="E7" t="s">
         <v>32</v>
       </c>
@@ -1272,7 +1339,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="5:9">
+    <row r="8" spans="5:9" x14ac:dyDescent="0.15">
       <c r="E8" t="s">
         <v>33</v>
       </c>
@@ -1288,20 +1355,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D7:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="9.5" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:8">
+    <row r="7" spans="4:8" x14ac:dyDescent="0.15">
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1312,7 +1379,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="4:8">
+    <row r="8" spans="4:8" x14ac:dyDescent="0.15">
       <c r="D8" s="2" t="s">
         <v>49</v>
       </c>
@@ -1323,7 +1390,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="4:8">
+    <row r="9" spans="4:8" x14ac:dyDescent="0.15">
       <c r="D9" s="2">
         <v>5.15</v>
       </c>
@@ -1331,7 +1398,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="4:8">
+    <row r="10" spans="4:8" x14ac:dyDescent="0.15">
       <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
@@ -1339,7 +1406,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="4:8">
+    <row r="11" spans="4:8" x14ac:dyDescent="0.15">
       <c r="D11" s="2" t="s">
         <v>43</v>
       </c>
@@ -1350,7 +1417,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="4:8">
+    <row r="12" spans="4:8" x14ac:dyDescent="0.15">
       <c r="D12" s="2" t="s">
         <v>44</v>
       </c>
@@ -1369,14 +1436,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D3:O62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="D3:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="5" max="5" width="54.75" customWidth="1"/>
     <col min="6" max="6" width="15.625" customWidth="1"/>
@@ -1388,7 +1455,7 @@
     <col min="15" max="15" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:10">
+    <row r="3" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D3" s="7" t="s">
         <v>79</v>
       </c>
@@ -1396,14 +1463,14 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="4:10">
+    <row r="4" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="4:10">
+    <row r="5" spans="4:10" x14ac:dyDescent="0.15">
       <c r="E5" t="s">
         <v>127</v>
       </c>
@@ -1415,7 +1482,7 @@
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="4:10">
+    <row r="6" spans="4:10" x14ac:dyDescent="0.15">
       <c r="E6" t="s">
         <v>136</v>
       </c>
@@ -1430,7 +1497,7 @@
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="4:10">
+    <row r="7" spans="4:10" x14ac:dyDescent="0.15">
       <c r="E7" t="s">
         <v>73</v>
       </c>
@@ -1442,14 +1509,14 @@
       </c>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="4:10">
+    <row r="8" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D8" t="s">
         <v>84</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="4:10">
+    <row r="9" spans="4:10" x14ac:dyDescent="0.15">
       <c r="E9" t="s">
         <v>65</v>
       </c>
@@ -1461,7 +1528,7 @@
       </c>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="4:10">
+    <row r="10" spans="4:10" x14ac:dyDescent="0.15">
       <c r="E10" t="s">
         <v>130</v>
       </c>
@@ -1473,7 +1540,7 @@
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="4:10">
+    <row r="11" spans="4:10" x14ac:dyDescent="0.15">
       <c r="E11" t="s">
         <v>75</v>
       </c>
@@ -1485,14 +1552,14 @@
       </c>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="4:10">
+    <row r="12" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D12" t="s">
         <v>7</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="4:10">
+    <row r="13" spans="4:10" x14ac:dyDescent="0.15">
       <c r="E13" t="s">
         <v>8</v>
       </c>
@@ -1504,7 +1571,7 @@
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="4:10">
+    <row r="14" spans="4:10" x14ac:dyDescent="0.15">
       <c r="E14" t="s">
         <v>96</v>
       </c>
@@ -1516,14 +1583,14 @@
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="4:10">
+    <row r="15" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D15" t="s">
         <v>10</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="4:10">
+    <row r="16" spans="4:10" x14ac:dyDescent="0.15">
       <c r="E16" t="s">
         <v>133</v>
       </c>
@@ -1535,7 +1602,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="4:9">
+    <row r="17" spans="4:9" x14ac:dyDescent="0.15">
       <c r="E17" t="s">
         <v>66</v>
       </c>
@@ -1547,7 +1614,7 @@
       </c>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="4:9">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.15">
       <c r="E18" t="s">
         <v>30</v>
       </c>
@@ -1559,7 +1626,7 @@
       </c>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="4:9">
+    <row r="19" spans="4:9" x14ac:dyDescent="0.15">
       <c r="E19" t="s">
         <v>75</v>
       </c>
@@ -1571,14 +1638,14 @@
       </c>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="4:9">
+    <row r="20" spans="4:9" x14ac:dyDescent="0.15">
       <c r="D20" t="s">
         <v>12</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="4:9">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.15">
       <c r="E21" t="s">
         <v>67</v>
       </c>
@@ -1590,7 +1657,7 @@
       </c>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="4:9">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.15">
       <c r="E22" t="s">
         <v>68</v>
       </c>
@@ -1602,14 +1669,14 @@
       </c>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="4:9">
+    <row r="23" spans="4:9" x14ac:dyDescent="0.15">
       <c r="D23" t="s">
         <v>82</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="4:9">
+    <row r="24" spans="4:9" x14ac:dyDescent="0.15">
       <c r="E24" t="s">
         <v>138</v>
       </c>
@@ -1621,7 +1688,7 @@
       </c>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="4:9">
+    <row r="25" spans="4:9" x14ac:dyDescent="0.15">
       <c r="E25" t="s">
         <v>139</v>
       </c>
@@ -1633,14 +1700,14 @@
       </c>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="4:9">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.15">
       <c r="D26" t="s">
         <v>83</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="4:9">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.15">
       <c r="E27" t="s">
         <v>26</v>
       </c>
@@ -1652,14 +1719,14 @@
       </c>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="4:9">
+    <row r="28" spans="4:9" x14ac:dyDescent="0.15">
       <c r="D28" t="s">
         <v>94</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="4:9">
+    <row r="29" spans="4:9" x14ac:dyDescent="0.15">
       <c r="E29" t="s">
         <v>78</v>
       </c>
@@ -1671,7 +1738,7 @@
       </c>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="4:9">
+    <row r="30" spans="4:9" x14ac:dyDescent="0.15">
       <c r="E30" t="s">
         <v>75</v>
       </c>
@@ -1683,14 +1750,14 @@
       </c>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="4:9">
+    <row r="31" spans="4:9" x14ac:dyDescent="0.15">
       <c r="D31" t="s">
         <v>28</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="4:9">
+    <row r="32" spans="4:9" x14ac:dyDescent="0.15">
       <c r="E32" t="s">
         <v>29</v>
       </c>
@@ -1701,19 +1768,19 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="4:8">
+    <row r="38" spans="4:8" x14ac:dyDescent="0.15">
       <c r="D38" s="7" t="s">
         <v>80</v>
       </c>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="4:8">
+    <row r="39" spans="4:8" x14ac:dyDescent="0.15">
       <c r="D39" t="s">
         <v>81</v>
       </c>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="4:8">
+    <row r="40" spans="4:8" x14ac:dyDescent="0.15">
       <c r="E40" t="s">
         <v>89</v>
       </c>
@@ -1724,7 +1791,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="4:8">
+    <row r="41" spans="4:8" x14ac:dyDescent="0.15">
       <c r="E41" t="s">
         <v>87</v>
       </c>
@@ -1735,7 +1802,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="4:8">
+    <row r="42" spans="4:8" x14ac:dyDescent="0.15">
       <c r="E42" t="s">
         <v>18</v>
       </c>
@@ -1746,13 +1813,13 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="4:8">
+    <row r="43" spans="4:8" x14ac:dyDescent="0.15">
       <c r="D43" t="s">
         <v>103</v>
       </c>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="4:8">
+    <row r="44" spans="4:8" x14ac:dyDescent="0.15">
       <c r="E44" t="s">
         <v>144</v>
       </c>
@@ -1763,147 +1830,153 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="4:8">
-      <c r="E45" t="s">
+    <row r="45" spans="4:8" ht="126.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E45" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="E46" t="s">
         <v>70</v>
-      </c>
-      <c r="F45" t="s">
-        <v>76</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="46" spans="4:8">
-      <c r="E46" t="s">
-        <v>71</v>
       </c>
       <c r="F46" t="s">
         <v>76</v>
       </c>
       <c r="H46" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="E47" t="s">
+        <v>71</v>
+      </c>
+      <c r="F47" t="s">
+        <v>76</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="4:8">
-      <c r="D47" t="s">
+    <row r="48" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="D48" t="s">
         <v>104</v>
       </c>
-      <c r="H47" s="3"/>
-    </row>
-    <row r="48" spans="4:8" ht="67.5">
-      <c r="E48" s="8" t="s">
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="4:8" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="E49" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="H48" s="3"/>
-    </row>
-    <row r="49" spans="4:8">
-      <c r="E49" t="s">
+      <c r="H49" s="3"/>
+    </row>
+    <row r="50" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="E50" t="s">
         <v>85</v>
       </c>
-      <c r="H49" s="3"/>
-    </row>
-    <row r="50" spans="4:8">
-      <c r="E50" t="s">
+      <c r="H50" s="3"/>
+    </row>
+    <row r="51" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="E51" t="s">
         <v>86</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F51" t="s">
         <v>120</v>
       </c>
-      <c r="H50" s="3" t="s">
+      <c r="H51" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="4:8">
-      <c r="D51" t="s">
+    <row r="52" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="D52" t="s">
         <v>105</v>
       </c>
-      <c r="H51" s="3"/>
-    </row>
-    <row r="52" spans="4:8">
-      <c r="E52" t="s">
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="E53" t="s">
         <v>90</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F53" t="s">
         <v>120</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="H53" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="4:8">
-      <c r="D53" t="s">
+    <row r="54" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="D54" t="s">
         <v>121</v>
       </c>
-      <c r="H53" s="3"/>
-    </row>
-    <row r="54" spans="4:8">
-      <c r="E54" t="s">
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="E55" t="s">
         <v>91</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F55" t="s">
         <v>120</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="H55" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="4:8">
-      <c r="D55" t="s">
+    <row r="56" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="D56" t="s">
         <v>122</v>
       </c>
-      <c r="H55" s="3"/>
-    </row>
-    <row r="56" spans="4:8">
-      <c r="E56" t="s">
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="E57" t="s">
         <v>92</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F57" t="s">
         <v>120</v>
       </c>
-      <c r="H56" s="3" t="s">
+      <c r="H57" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="4:8">
-      <c r="D57" t="s">
+    <row r="58" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="D58" t="s">
         <v>123</v>
       </c>
-      <c r="H57" s="3"/>
-    </row>
-    <row r="58" spans="4:8">
-      <c r="E58" t="s">
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="E59" t="s">
         <v>93</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F59" t="s">
         <v>120</v>
       </c>
-      <c r="H58" s="3" t="s">
+      <c r="H59" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="4:8">
-      <c r="D59" t="s">
+    <row r="60" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="D60" t="s">
         <v>124</v>
       </c>
-      <c r="H59" s="3"/>
-    </row>
-    <row r="60" spans="4:8">
-      <c r="E60" t="s">
+      <c r="H60" s="3"/>
+    </row>
+    <row r="61" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="E61" t="s">
         <v>93</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F61" t="s">
         <v>120</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="H61" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="4:8">
-      <c r="H61" s="3"/>
-    </row>
-    <row r="62" spans="4:8">
+    <row r="62" spans="4:8" x14ac:dyDescent="0.15">
       <c r="H62" s="3"/>
+    </row>
+    <row r="63" spans="4:8" x14ac:dyDescent="0.15">
+      <c r="H63" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1913,86 +1986,86 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="F9:F30"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="9" spans="6:6">
+    <row r="9" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="6:6">
+    <row r="11" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="6:6">
+    <row r="12" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="6:6">
+    <row r="13" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="6:6">
+    <row r="14" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="6:6">
+    <row r="15" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F15" s="10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="6:6">
+    <row r="16" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F16" s="10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="6:6">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="6:6">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="6:6">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F21" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="6:6">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="6:6">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="6:6">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F27" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="6:6">
+    <row r="30" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F30" t="s">
         <v>118</v>
       </c>

</xml_diff>